<commit_message>
docs: update sheets for 2023-09
</commit_message>
<xml_diff>
--- a/账户明细.xlsx
+++ b/账户明细.xlsx
@@ -607,7 +607,7 @@
         <v>601318</v>
       </c>
       <c r="C2" s="20" t="n">
-        <v>50.2</v>
+        <v>50.33</v>
       </c>
       <c r="D2" s="21" t="n">
         <v>100</v>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C3" s="20" t="n">
-        <v>35.38</v>
+        <v>33.57</v>
       </c>
       <c r="D3" s="21" t="n">
         <v>800</v>
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="C4" s="20" t="n">
-        <v>50.3</v>
+        <v>48.58</v>
       </c>
       <c r="D4" s="21" t="n">
         <v>700</v>
@@ -693,7 +693,7 @@
         </is>
       </c>
       <c r="C5" s="20" t="n">
-        <v>54.5</v>
+        <v>53.12</v>
       </c>
       <c r="D5" s="21" t="n">
         <v>720</v>
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="C6" s="20" t="n">
-        <v>30.93</v>
+        <v>30.92</v>
       </c>
       <c r="D6" s="21" t="n">
         <v>600</v>
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="C7" s="20" t="n">
-        <v>38.26</v>
+        <v>40.05</v>
       </c>
       <c r="D7" s="21" t="n">
         <v>640</v>
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="C8" s="1" t="n">
-        <v>26.6</v>
+        <v>26.29</v>
       </c>
       <c r="D8" s="21" t="n">
         <v>200</v>
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="C9" s="20" t="n">
-        <v>23.79</v>
+        <v>25.87</v>
       </c>
       <c r="D9" s="21" t="n">
         <v>200</v>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="C10" s="20" t="n">
-        <v>24.72</v>
+        <v>25.04</v>
       </c>
       <c r="D10" s="21" t="n">
         <v>1200</v>
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="C11" s="20" t="n">
-        <v>139.53</v>
+        <v>133.8</v>
       </c>
       <c r="D11" s="21" t="n">
         <v>100</v>
@@ -883,7 +883,7 @@
         </is>
       </c>
       <c r="C12" s="20" t="n">
-        <v>165.72</v>
+        <v>159.92</v>
       </c>
       <c r="D12" s="21" t="n">
         <v>100</v>
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="C13" s="20" t="n">
-        <v>238.08</v>
+        <v>227</v>
       </c>
       <c r="D13" s="21" t="n">
         <v>100</v>
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="C14" s="20" t="n">
-        <v>0.836</v>
+        <v>0.801</v>
       </c>
       <c r="D14" s="21" t="n">
         <v>12700</v>
@@ -961,7 +961,7 @@
         </is>
       </c>
       <c r="C15" s="20" t="n">
-        <v>10.68</v>
+        <v>10.42</v>
       </c>
       <c r="D15" s="21" t="n">
         <v>1568</v>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="C16" s="20" t="n">
-        <v>26.03</v>
+        <v>26.6</v>
       </c>
       <c r="D16" s="21" t="n">
         <v>900</v>
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="C17" s="20" t="n">
-        <v>26.79</v>
+        <v>26.71</v>
       </c>
       <c r="D17" s="21" t="n">
         <v>800</v>
@@ -1043,7 +1043,7 @@
         </is>
       </c>
       <c r="C18" s="20" t="n">
-        <v>16.3</v>
+        <v>16.05</v>
       </c>
       <c r="D18" s="21" t="n">
         <v>1000</v>
@@ -1069,7 +1069,7 @@
         </is>
       </c>
       <c r="C19" s="20" t="n">
-        <v>33.73</v>
+        <v>34.24</v>
       </c>
       <c r="D19" s="21" t="n">
         <v>600</v>
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="C20" s="20" t="n">
-        <v>36.96</v>
+        <v>36.71</v>
       </c>
       <c r="D20" s="21" t="n">
         <v>300</v>
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="C21" s="20" t="n">
-        <v>30.56</v>
+        <v>27.42</v>
       </c>
       <c r="D21" s="21" t="n">
         <v>200</v>
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="C22" s="1" t="n">
-        <v>114.5</v>
+        <v>109.3</v>
       </c>
       <c r="D22" s="21" t="n">
         <v>100</v>
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="C23" s="20" t="n">
-        <v>3.893</v>
+        <v>3.817</v>
       </c>
       <c r="D23" s="21" t="n">
         <v>200</v>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="C24" s="20" t="n">
-        <v>4.508</v>
+        <v>4.561</v>
       </c>
       <c r="D24" s="21" t="n">
         <v>1400</v>
@@ -1352,7 +1352,7 @@
         <v>601318</v>
       </c>
       <c r="C2" s="20" t="n">
-        <v>50.2</v>
+        <v>50.33</v>
       </c>
       <c r="D2" s="21" t="n">
         <v>200</v>
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="C3" s="20" t="n">
-        <v>35.38</v>
+        <v>33.57</v>
       </c>
       <c r="D3" s="21" t="n">
         <v>1400</v>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="C4" s="20" t="n">
-        <v>50.3</v>
+        <v>48.58</v>
       </c>
       <c r="D4" s="21" t="n">
         <v>1200</v>
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="C5" s="20" t="n">
-        <v>54.5</v>
+        <v>53.12</v>
       </c>
       <c r="D5" s="21" t="n">
         <v>900</v>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="C6" s="20" t="n">
-        <v>30.93</v>
+        <v>30.92</v>
       </c>
       <c r="D6" s="21" t="n">
         <v>1000</v>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="C7" s="20" t="n">
-        <v>38.26</v>
+        <v>40.05</v>
       </c>
       <c r="D7" s="21" t="n">
         <v>1240</v>
@@ -1520,7 +1520,7 @@
         </is>
       </c>
       <c r="C8" s="20" t="n">
-        <v>26.6</v>
+        <v>26.29</v>
       </c>
       <c r="D8" s="21" t="n">
         <v>900</v>
@@ -1546,7 +1546,7 @@
         </is>
       </c>
       <c r="C9" s="20" t="n">
-        <v>23.79</v>
+        <v>25.87</v>
       </c>
       <c r="D9" s="21" t="n">
         <v>200</v>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="C10" s="20" t="n">
-        <v>24.72</v>
+        <v>25.04</v>
       </c>
       <c r="D10" s="21" t="n">
         <v>2040</v>
@@ -1598,7 +1598,7 @@
         </is>
       </c>
       <c r="C11" s="20" t="n">
-        <v>139.53</v>
+        <v>133.8</v>
       </c>
       <c r="D11" s="21" t="n">
         <v>300</v>
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="C12" s="20" t="n">
-        <v>238.08</v>
+        <v>227</v>
       </c>
       <c r="D12" s="21" t="n">
         <v>100</v>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="C13" s="20" t="n">
-        <v>165.72</v>
+        <v>159.92</v>
       </c>
       <c r="D13" s="21" t="n">
         <v>100</v>
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="C14" s="20" t="n">
-        <v>258.31</v>
+        <v>246.31</v>
       </c>
       <c r="D14" s="21" t="n">
         <v>140</v>
@@ -1706,7 +1706,7 @@
         </is>
       </c>
       <c r="C15" s="20" t="n">
-        <v>0.836</v>
+        <v>0.801</v>
       </c>
       <c r="D15" s="21" t="n">
         <v>21900</v>
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="C16" s="20" t="n">
-        <v>39.99</v>
+        <v>39.3</v>
       </c>
       <c r="D16" s="21" t="n">
         <v>400</v>
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="C17" s="20" t="n">
-        <v>10.68</v>
+        <v>10.42</v>
       </c>
       <c r="D17" s="21" t="n">
         <v>2668</v>
@@ -1788,7 +1788,7 @@
         </is>
       </c>
       <c r="C18" s="20" t="n">
-        <v>26.03</v>
+        <v>26.6</v>
       </c>
       <c r="D18" s="21" t="n">
         <v>1500</v>
@@ -1814,7 +1814,7 @@
         </is>
       </c>
       <c r="C19" s="20" t="n">
-        <v>26.79</v>
+        <v>26.71</v>
       </c>
       <c r="D19" s="21" t="n">
         <v>1400</v>
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="C20" s="20" t="n">
-        <v>16.3</v>
+        <v>16.05</v>
       </c>
       <c r="D20" s="21" t="n">
         <v>1800</v>
@@ -1866,7 +1866,7 @@
         </is>
       </c>
       <c r="C21" s="20" t="n">
-        <v>33.73</v>
+        <v>34.24</v>
       </c>
       <c r="D21" s="21" t="n">
         <v>1100</v>
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="C22" s="20" t="n">
-        <v>36.96</v>
+        <v>36.71</v>
       </c>
       <c r="D22" s="21" t="n">
         <v>400</v>
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="C23" s="20" t="n">
-        <v>30.56</v>
+        <v>27.42</v>
       </c>
       <c r="D23" s="21" t="n">
         <v>200</v>
@@ -1948,7 +1948,7 @@
         </is>
       </c>
       <c r="C24" s="20" t="n">
-        <v>114.5</v>
+        <v>109.3</v>
       </c>
       <c r="D24" s="21" t="n">
         <v>300</v>
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="C25" s="20" t="n">
-        <v>3.893</v>
+        <v>3.817</v>
       </c>
       <c r="D25" s="21" t="n">
         <v>2800</v>
@@ -2008,7 +2008,7 @@
         </is>
       </c>
       <c r="C26" s="20" t="n">
-        <v>1.128</v>
+        <v>1.1</v>
       </c>
       <c r="D26" s="21" t="n">
         <v>500</v>
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="C27" s="20" t="n">
-        <v>4.508</v>
+        <v>4.561</v>
       </c>
       <c r="D27" s="21" t="n">
         <v>4700</v>

</xml_diff>